<commit_message>
Formulas & functions lesson classwork
</commit_message>
<xml_diff>
--- a/Excel - Formulas & Functions/Day1PM_learner_WorkshopData.xlsx
+++ b/Excel - Formulas & Functions/Day1PM_learner_WorkshopData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27927"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramlal\Documents\LaFosseAssociatesProgramme\DeepDive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42980713-35D6-4F1E-9441-C5437DAF8D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA9C3BFA-F8A5-40CC-B783-F3B32CF12EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C9C4612E-932B-4A27-B978-84C071736509}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1018" r:id="rId2"/>
+    <pivotCache cacheId="6034" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="44">
   <si>
     <t>SaleID</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Kurtosis</t>
   </si>
   <si>
     <t>Notebook</t>
@@ -1483,7 +1486,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3BC7BD0-FF83-49AF-9919-72125FE1CCA4}" name="PivotTable1" cacheId="1018" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3BC7BD0-FF83-49AF-9919-72125FE1CCA4}" name="PivotTable1" cacheId="6034" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="K3:L8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -1543,7 +1546,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B8A82143-E3EA-4301-84BC-AD56B3D53DEA}" name="PivotTable2" cacheId="1018" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B8A82143-E3EA-4301-84BC-AD56B3D53DEA}" name="PivotTable2" cacheId="6034" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="K11:R23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
@@ -1978,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9B0860-4495-47C7-9213-747D7C9160FF}">
   <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -3529,7 +3532,7 @@
         <v>Low</v>
       </c>
     </row>
-    <row r="40" spans="1:22">
+    <row r="40" spans="1:22" ht="15">
       <c r="A40">
         <v>19</v>
       </c>
@@ -3556,6 +3559,13 @@
       </c>
       <c r="I40">
         <v>4</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L40">
+        <f>KURT(F2:F51)</f>
+        <v>4.6162104880434587</v>
       </c>
       <c r="V40" t="str">
         <f t="shared" si="0"/>
@@ -3573,10 +3583,10 @@
         <v>204</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E41" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F41">
         <v>18</v>
@@ -3606,10 +3616,10 @@
         <v>204</v>
       </c>
       <c r="D42" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F42">
         <v>16</v>
@@ -3672,10 +3682,10 @@
         <v>204</v>
       </c>
       <c r="D44" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E44" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F44">
         <v>14</v>
@@ -3705,10 +3715,10 @@
         <v>204</v>
       </c>
       <c r="D45" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E45" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F45">
         <v>12</v>
@@ -3738,10 +3748,10 @@
         <v>204</v>
       </c>
       <c r="D46" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E46" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F46">
         <v>10</v>
@@ -3771,10 +3781,10 @@
         <v>210</v>
       </c>
       <c r="D47" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" t="s">
         <v>42</v>
-      </c>
-      <c r="E47" t="s">
-        <v>41</v>
       </c>
       <c r="F47">
         <v>10</v>
@@ -3804,10 +3814,10 @@
         <v>210</v>
       </c>
       <c r="D48" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" t="s">
         <v>42</v>
-      </c>
-      <c r="E48" t="s">
-        <v>41</v>
       </c>
       <c r="F48">
         <v>9</v>
@@ -3837,10 +3847,10 @@
         <v>210</v>
       </c>
       <c r="D49" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" t="s">
         <v>42</v>
-      </c>
-      <c r="E49" t="s">
-        <v>41</v>
       </c>
       <c r="F49">
         <v>8</v>
@@ -3870,10 +3880,10 @@
         <v>210</v>
       </c>
       <c r="D50" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" t="s">
         <v>42</v>
-      </c>
-      <c r="E50" t="s">
-        <v>41</v>
       </c>
       <c r="F50">
         <v>7</v>
@@ -3903,10 +3913,10 @@
         <v>210</v>
       </c>
       <c r="D51" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" t="s">
         <v>42</v>
-      </c>
-      <c r="E51" t="s">
-        <v>41</v>
       </c>
       <c r="F51">
         <v>5</v>

</xml_diff>